<commit_message>
finished olkina's testing first lab
</commit_message>
<xml_diff>
--- a/Тестирование/Моя/1/Лист Microsoft Excel.xlsx
+++ b/Тестирование/Моя/1/Лист Microsoft Excel.xlsx
@@ -269,7 +269,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -303,6 +303,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -385,11 +389,11 @@
   </sheetPr>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L61" activeCellId="0" sqref="L61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P44" activeCellId="0" sqref="P44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -546,7 +550,7 @@
         <v>18</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,7 +631,7 @@
       </c>
       <c r="J11" s="5" t="n">
         <f aca="false">J5+J8</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,7 +691,7 @@
       </c>
       <c r="J14" s="5" t="n">
         <f aca="false">J12*LOG(J11,2)</f>
-        <v>135.514401580475</v>
+        <v>67.7572007902374</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,7 +711,7 @@
       </c>
       <c r="J15" s="5" t="n">
         <f aca="false">J14/J13</f>
-        <v>0.870974447086231</v>
+        <v>0.435487223543116</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,7 +822,7 @@
       </c>
       <c r="J21" s="5" t="n">
         <f aca="false">J15^2*J13</f>
-        <v>118.029580988776</v>
+        <v>29.5073952471939</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,7 +1022,7 @@
         <v>18</v>
       </c>
       <c r="J32" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,7 +1095,7 @@
       </c>
       <c r="J35" s="5" t="n">
         <f aca="false">J29+J32</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,7 +1155,7 @@
       </c>
       <c r="J38" s="5" t="n">
         <f aca="false">J36*LOG(J35,2)</f>
-        <v>97.4581119064011</v>
+        <v>48.7290559532006</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,7 +1169,7 @@
       </c>
       <c r="J39" s="5" t="n">
         <f aca="false">J38/J37</f>
-        <v>0.676792443794452</v>
+        <v>0.338396221897226</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,7 +1268,7 @@
       </c>
       <c r="J45" s="5" t="n">
         <f aca="false">J39^2*J37</f>
-        <v>65.9589137247264</v>
+        <v>16.4897284311816</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1488,7 @@
         <v>18</v>
       </c>
       <c r="J57" s="8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,17 +1563,17 @@
       </c>
       <c r="J60" s="5" t="n">
         <f aca="false">J54+J57</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="0" t="n">
+      <c r="C61" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G61" s="5"/>
@@ -1586,10 +1590,10 @@
       <c r="A62" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="C62" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G62" s="5"/>
@@ -1606,10 +1610,10 @@
       <c r="A63" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C63" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G63" s="5"/>
@@ -1619,7 +1623,7 @@
       </c>
       <c r="J63" s="5" t="n">
         <f aca="false">J61*LOG(J60,2)</f>
-        <v>97.4581119064011</v>
+        <v>48.7290559532006</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,7 +1635,7 @@
       </c>
       <c r="J64" s="5" t="n">
         <f aca="false">J63/J62</f>
-        <v>0.738319029593948</v>
+        <v>0.369159514796974</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,7 +1732,7 @@
       </c>
       <c r="J70" s="5" t="n">
         <f aca="false">J64^2*J62</f>
-        <v>71.9551786087924</v>
+        <v>17.9887946521981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>